<commit_message>
Updated on conflict resolution.
</commit_message>
<xml_diff>
--- a/clones_validation/CM_conflicts.xlsx
+++ b/clones_validation/CM_conflicts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27000" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="51200" windowHeight="27000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CM_conflicts.csv" sheetId="1" r:id="rId1"/>
@@ -2180,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3688,7 +3688,7 @@
         <v>554</v>
       </c>
       <c r="T27" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="U27" t="s">
         <v>340</v>
@@ -3736,7 +3736,7 @@
         <v>554</v>
       </c>
       <c r="T28" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="U28" t="s">
         <v>340</v>
@@ -3946,7 +3946,7 @@
         <v>554</v>
       </c>
       <c r="T32" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="U32" t="s">
         <v>355</v>

</xml_diff>

<commit_message>
Resolved the conflicts in 345 clone pairs.
</commit_message>
<xml_diff>
--- a/clones_validation/CM_conflicts.xlsx
+++ b/clones_validation/CM_conflicts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaiyong/Documents/StackoverflowChecker/clones_validation/"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3005" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="605">
   <si>
     <t>good</t>
   </si>
@@ -1884,17 +1884,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2180,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3952,7 +3942,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -4011,8 +4001,14 @@
       <c r="S33" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" t="s">
+        <v>4</v>
+      </c>
+      <c r="U33" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -4071,8 +4067,14 @@
       <c r="S34" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" t="s">
+        <v>4</v>
+      </c>
+      <c r="U34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4113,8 +4115,14 @@
       <c r="S35" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" t="s">
+        <v>15</v>
+      </c>
+      <c r="U35" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4155,8 +4163,14 @@
       <c r="S36" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" t="s">
+        <v>15</v>
+      </c>
+      <c r="U36" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -4197,8 +4211,14 @@
       <c r="S37" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" t="s">
+        <v>4</v>
+      </c>
+      <c r="U37" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -4257,8 +4277,14 @@
       <c r="S38" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4299,8 +4325,14 @@
       <c r="S39" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T39" t="s">
+        <v>103</v>
+      </c>
+      <c r="U39" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -4359,8 +4391,14 @@
       <c r="S40" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T40" t="s">
+        <v>4</v>
+      </c>
+      <c r="U40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4401,8 +4439,14 @@
       <c r="S41" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41" t="s">
+        <v>33</v>
+      </c>
+      <c r="U41" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -4443,8 +4487,14 @@
       <c r="S42" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T42" t="s">
+        <v>4</v>
+      </c>
+      <c r="U42" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4485,8 +4535,14 @@
       <c r="S43" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T43" t="s">
+        <v>4</v>
+      </c>
+      <c r="U43" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4527,8 +4583,14 @@
       <c r="S44" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T44" t="s">
+        <v>33</v>
+      </c>
+      <c r="U44" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4569,8 +4631,14 @@
       <c r="S45" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T45" t="s">
+        <v>53</v>
+      </c>
+      <c r="U45" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4629,8 +4697,14 @@
       <c r="S46" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T46" t="s">
+        <v>4</v>
+      </c>
+      <c r="U46" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>263</v>
       </c>
@@ -4671,8 +4745,14 @@
       <c r="S47" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T47" t="s">
+        <v>4</v>
+      </c>
+      <c r="U47" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4713,8 +4793,14 @@
       <c r="S48" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T48" t="s">
+        <v>4</v>
+      </c>
+      <c r="U48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -4755,8 +4841,14 @@
       <c r="S49" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T49" t="s">
+        <v>4</v>
+      </c>
+      <c r="U49" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -4797,8 +4889,14 @@
       <c r="S50" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T50" t="s">
+        <v>4</v>
+      </c>
+      <c r="U50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -4839,8 +4937,14 @@
       <c r="S51" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T51" t="s">
+        <v>15</v>
+      </c>
+      <c r="U51" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4881,8 +4985,14 @@
       <c r="S52" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T52" t="s">
+        <v>4</v>
+      </c>
+      <c r="U52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -4923,8 +5033,14 @@
       <c r="S53" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T53" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -4965,8 +5081,14 @@
       <c r="S54" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T54" t="s">
+        <v>4</v>
+      </c>
+      <c r="U54" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -5025,8 +5147,14 @@
       <c r="S55" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T55" t="s">
+        <v>4</v>
+      </c>
+      <c r="U55" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -5086,7 +5214,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -5146,7 +5274,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -5206,7 +5334,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -5248,7 +5376,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -5308,7 +5436,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -5368,7 +5496,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -5428,7 +5556,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -5488,7 +5616,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -21519,6 +21647,9 @@
     <sortCondition ref="Q2:Q346"/>
   </sortState>
   <conditionalFormatting sqref="Q2:Q346">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",Q2)))</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -21529,9 +21660,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",Q2)))</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>